<commit_message>
Do not add space between text nodes
</commit_message>
<xml_diff>
--- a/tests/resources/xlsx/one_sheet_with_shared_strings_containing_text_and_hyperlink_in_same_cell.xlsx
+++ b/tests/resources/xlsx/one_sheet_with_shared_strings_containing_text_and_hyperlink_in_same_cell.xlsx
@@ -29,7 +29,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>go to </t>
+      <t xml:space="preserve">go to </t>
     </r>
     <r>
       <rPr>
@@ -48,7 +48,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t> please</t>
+      <t xml:space="preserve"> please</t>
     </r>
   </si>
 </sst>

</xml_diff>

<commit_message>
Do not add space between text nodes (#401)
</commit_message>
<xml_diff>
--- a/tests/resources/xlsx/one_sheet_with_shared_strings_containing_text_and_hyperlink_in_same_cell.xlsx
+++ b/tests/resources/xlsx/one_sheet_with_shared_strings_containing_text_and_hyperlink_in_same_cell.xlsx
@@ -29,7 +29,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>go to </t>
+      <t xml:space="preserve">go to </t>
     </r>
     <r>
       <rPr>
@@ -48,7 +48,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t> please</t>
+      <t xml:space="preserve"> please</t>
     </r>
   </si>
 </sst>

</xml_diff>